<commit_message>
revised fontmaker and Russian hellscreiber fonts
</commit_message>
<xml_diff>
--- a/fontmaker.xlsx
+++ b/fontmaker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="600" windowWidth="24720" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="1920" yWindow="340" windowWidth="16500" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,174 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
-  <si>
-    <t>00000000000000-00111111111000-00110000011110-00110000011100-00110000011000-00110000011000-00000000000000</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+  <si>
+    <t>00000000000000-00000000001100-00000000001100-00111111111100-00110011000000-00011110000000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111100-00110011000000-00011110000000-00000000000000-00111111111100-00000000000000</t>
+  </si>
+  <si>
+    <t>Ф</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000000000000-00000000000000-00000000000000-00110000000000-00110000000000-00000000000000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00000000000000-00000000000000-01100000000000-00110000000000-00000000000000-00000000000000</t>
+  </si>
+  <si>
+    <t>Ч</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000000000000-00000000111100-00000001100000-00000001100000-00000001100000-00111111111100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111100-00110011000000-00110011000000-00110011000000-00011110000000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00110011001100-00110011001100-00110011001100-00011011011000-00001111110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111100-00000011000000-00001100110000-00110000001100-00001111110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111001111000-00001111001100-00000011001100-00000011001100-00111111111100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00011000011000-00110011001100-00110011001100-00110011001100-00011100111000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111000001100-00000111111100-00000000001100-00000000001100-00111111111100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111100-00000000001100-00000000001100-00000000001100-00111111111100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111100-00110000000000-00110000000000-01110000000000-00111111111100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111100-00110000000000-00111111111100-01110000000000-00111111111100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111100-00110000000000-00111111111100-00110000000000-00111111111100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00000001111000-00000011001100-00111111111100-00000011001100-00000001111000-00000000000000</t>
+  </si>
+  <si>
+    <t>Д</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000000000000-00110000001100-00111111111100-00110011001100-00110011001100-00011110001100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00110000001100-00111111111100-00110000001100-0000000001100-00000000011100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111100-00001110000000-00000011100000-00000000111000-00111111111100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111110000-00011000000110-00000110001100-00000001100110-00111111110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-01111000000000-001101110001100-00110000111100-00111111111100-01110000001100-00000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Types a 1 or 0 into the grid below; 1 becomes a black pixel and zero a while pixel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copy result from above cell, then paste-special-value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Р</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>С</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Х</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ш</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Щ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ь</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Э</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ю</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Я</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Т</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>У</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ъ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ы</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^^</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>comma</t>
@@ -182,10 +347,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Д</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Е</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -218,248 +379,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>00000000000000-00001100011100-01101100111100-01101101101100-01101111001100-00001110001100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000111111100-00110110001100-01100110001100-00110110001100-00000110001100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000111111100-00000110001100-00110110001100-01100110001100-00000110001100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000111001100-01101101101100-00111101101100-01101101101100-00001100111000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000011100110-00110110110110-01100110110110-00110110110110-00000110011100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000111001100-00001101101100-00111101101100-01101101101100-00001100111000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00110011001100-00111111111100-00110011001100-00110000001100-00011111111000-00000000000000</t>
-  </si>
-  <si>
     <t>00000000000000-00111100111100-00000011000000-00111111111100-00000011000000-00111100111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00111111111100-00000000001100-00111111111100-00000000001100-00111111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00111111111100-00000000001100-00111111111100-00000000001110-00111111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00111111111100-00110000000000-00110000000000-00110000000000-00111111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00001111111100-00001101101100-00111101101100-01101100001100-00001100001100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00001111111100-01101101101100-00111101101100-00001100001100-00001100001100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00111111110000-00110110111100-00110110110110-00110000110000-00110000110000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000011000000-01111111111100-00000110001100-00001100001100-00000000001100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000011111100-00110110000110-01100110000110-00110110110110-00000110111100-00000000000000</t>
-  </si>
-  <si>
-    <t>Т</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>У</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ф</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ъ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ы</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^^</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00000000000000-00000111111100-01101100110000-00001000110000-01101100110000-00000111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000111111100-01101100110000-00001000110000-00001100110000-00000111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00011110000000-00110011000000-01111111111100-00110011000000-00011110000000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00111111111100-00000000000100-00000000000100-00000000000110-00111111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00111111111110-00000011000000-00001111111000-00110000000110-00001111111000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00110000000000-00111111111110-00000001100110-00000001100110-00000000111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000111111100-00110000110000-01100000110000-00110000110000-00000111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000000111100-00110000001100-01100000001100-00110000001100-00000111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000111111100-01100000001100-00110000001100-01100000001100-00000111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00001111111100-00011000111000-00011011011000-00011100011000-00111111110000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00001111111100-00001100001100-00111100001100-01101100001100-00001111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00111111111100-00001101100000-00001101100000-00001101100000-00000111000000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00001100011100-00001100111100-00111101101100-01101111001100-00001110001100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00110111111100-01100011000000-00110001100000-00110000110000-01100111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000111111100-00000011000000-00110001100000-01100000110000-00000111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>Types a 1 or 0 into the grid below; 1 becomes a black pixel and zero a while pixel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Copy result from above cell, then paste-special-value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Р</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin P</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>С</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Х</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ш</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Щ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ь</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Э</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ю</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Я</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00000000000000-00111111111110-00000001100110-00000001100110-00000001100110-00000000111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00111111111110-00000001100110-00000000111100-00000000000000-00111111111110-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00011110011100-00110011110000-00110011000000-00110011000000-00111111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-01111111111100-01100000000000-01100000000000-01100000000000-01100000000000-00000000000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00000000000000-00001111111100-00110001100000-00110001100000-00001111111100-00000000000110-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000011111000-00110110001100-00000110001100-00110110001100-00000011111000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000111111100-00110000001100-00000000001100-00110000001100-00000111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000111111100-01100000011000-00110001110000-01100011000000-00000111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000000000000-00000000000000-00000000001100-00000000001100-00000000000000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000000000000-00000000000000-00000000001100-00000000001110-00000000000000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000011111100-00110111011000-01101110011000-00110111011000-00000011111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00001111111100-00110001100000-00011111111100-00011001101100-00011001101100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00111111111100-00110011001100-00110011001100-00110011001100-00110001111000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00110000011110-00110011110100-00111100000100-00111111111100-00110000000110-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00011000011000-00110011001100-00110011001100-00011100111000-00000000000000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00011011011000-00110011001100-00110011001100-00011111111000-00000000000000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00111111111100-00000001110000-00000111000000-00011100000000-00111111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00000000001100-01111111110000-01100000000000-01100000000000-01111111111100-00000000000000</t>
   </si>
 </sst>
 </file>
@@ -524,7 +444,38 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="8"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -881,22 +832,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K86"/>
+  <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A17" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24:K86"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A65" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="8" width="1.85546875" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -923,7 +873,7 @@
       </c>
       <c r="J3" s="2" t="str">
         <f>B21&amp;"-"&amp;C21&amp;"-"&amp;D21&amp;"-"&amp;E21&amp;"-"&amp;F21&amp;"-"&amp;G21&amp;"-"&amp;H21</f>
-        <v>00000000000000-00001100011100-01101100111100-01101101101100-01101111001100-00001110001100-00000000000000</v>
+        <v>00000000000000-00000000111100-00000001100000-00000001100000-00000001100000-00111111111100-00000000000000</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -935,7 +885,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -964,7 +914,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -978,13 +928,13 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1001,19 +951,19 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1027,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1039,7 +989,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1056,13 +1006,13 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1108,10 +1058,10 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1137,13 +1087,13 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1160,16 +1110,16 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1183,10 +1133,10 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1195,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1209,16 +1159,16 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1235,16 +1185,16 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1316,28 +1266,28 @@
     </row>
     <row r="21" spans="1:11" ht="185" customHeight="1">
       <c r="B21" s="3" t="str">
-        <f>B5&amp;B6&amp;B7&amp;B8&amp;B9&amp;B10&amp;B11&amp;B12&amp;B13&amp;B14&amp;B15&amp;B16&amp;B17&amp;B18</f>
+        <f>B18&amp;B17&amp;B16&amp;B15&amp;B14&amp;B13&amp;B12&amp;B11&amp;B10&amp;B9&amp;B8&amp;B7&amp;B6&amp;B5</f>
         <v>00000000000000</v>
       </c>
       <c r="C21" s="3" t="str">
-        <f t="shared" ref="C21:H21" si="0">C5&amp;C6&amp;C7&amp;C8&amp;C9&amp;C10&amp;C11&amp;C12&amp;C13&amp;C14&amp;C15&amp;C16&amp;C17&amp;C18</f>
-        <v>00001100011100</v>
+        <f t="shared" ref="C21:H21" si="0">C18&amp;C17&amp;C16&amp;C15&amp;C14&amp;C13&amp;C12&amp;C11&amp;C10&amp;C9&amp;C8&amp;C7&amp;C6&amp;C5</f>
+        <v>00000000111100</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>01101100111100</v>
+        <v>00000001100000</v>
       </c>
       <c r="E21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>01101101101100</v>
+        <v>00000001100000</v>
       </c>
       <c r="F21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>01101111001100</v>
+        <v>00000001100000</v>
       </c>
       <c r="G21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>00001110001100</v>
+        <v>00111111111100</v>
       </c>
       <c r="H21" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1346,503 +1296,423 @@
     </row>
     <row r="24" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J24" s="4" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>118</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J25" s="4" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J29" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>119</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J31" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J32" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="10:11" s="4" customFormat="1" ht="25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="10:10" s="4" customFormat="1" ht="25">
       <c r="J33" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="10:11" s="4" customFormat="1" ht="25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="10:10" s="4" customFormat="1" ht="25">
       <c r="J34" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="10:11" s="4" customFormat="1" ht="25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="10:10" s="4" customFormat="1" ht="25">
       <c r="J35" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="10:11" s="4" customFormat="1" ht="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="10:10" s="4" customFormat="1" ht="25">
       <c r="J36" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="10:11" s="4" customFormat="1" ht="25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="10:10" s="4" customFormat="1" ht="25">
       <c r="J37" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="10:11" s="4" customFormat="1" ht="25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="10:10" s="4" customFormat="1" ht="25">
       <c r="J38" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="10:11" s="4" customFormat="1" ht="25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="10:10" s="4" customFormat="1" ht="25">
       <c r="J39" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="10:11" s="4" customFormat="1" ht="25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="10:10" s="4" customFormat="1" ht="25">
       <c r="J40" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="10:11" s="4" customFormat="1" ht="25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="10:10" s="4" customFormat="1" ht="25">
       <c r="J41" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="10:11" s="4" customFormat="1" ht="25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="10:10" s="4" customFormat="1" ht="25">
       <c r="J42" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="10:11" s="4" customFormat="1" ht="25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="10:10" s="4" customFormat="1" ht="25">
       <c r="J43" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="10:11" s="4" customFormat="1" ht="25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="10:10" s="4" customFormat="1" ht="25">
       <c r="J44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K44" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="10:10" s="4" customFormat="1" ht="25">
+      <c r="J45" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="10:10" s="4" customFormat="1" ht="25">
+      <c r="J46" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="10:10" s="4" customFormat="1" ht="25">
+      <c r="J47" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="10:10" s="4" customFormat="1" ht="25">
+      <c r="J48" s="4" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="10:11" s="4" customFormat="1" ht="25">
-      <c r="J45" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K45" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="10:11" s="4" customFormat="1" ht="25">
-      <c r="J46" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="10:11" s="4" customFormat="1" ht="25">
-      <c r="J47" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="48" spans="10:11" s="4" customFormat="1" ht="25">
-      <c r="J48" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K48" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="49" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J49" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K49" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J50" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K50" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J51" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K51" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J52" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K52" s="4" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J53" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J54" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K54" s="4" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="10:11" s="4" customFormat="1" ht="25"/>
     <row r="56" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J56" s="4" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J57" s="4" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>121</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J58" s="4" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J59" s="4" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J60" s="4" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>122</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J61" s="4" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J62" s="4" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J63" s="4" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J64" s="4" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>125</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J65" s="4" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J66" s="4" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J67" s="4" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>126</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J68" s="4" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="K68" s="4" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J69" s="4" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="K69" s="4" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J70" s="4" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="K70" s="4" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
     </row>
     <row r="71" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J71" s="4" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J72" s="4" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="K72" s="4" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J73" s="4" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="K73" s="4" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
     </row>
     <row r="74" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J74" s="4" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="K74" s="4" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="75" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J75" s="4" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="K75" s="4" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J76" s="4" t="s">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="K76" s="4" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J77" s="4" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="K77" s="4" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
     </row>
     <row r="78" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J78" s="4" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="K78" s="4" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J79" s="4" t="s">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="K79" s="4" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J80" s="4" t="s">
-        <v>104</v>
+        <v>36</v>
       </c>
       <c r="K80" s="4" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J81" s="4" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="K81" s="4" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J82" s="4" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="K82" s="4" t="s">
-        <v>110</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J83" s="4" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="K83" s="4" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J84" s="4" t="s">
-        <v>106</v>
+        <v>38</v>
       </c>
       <c r="K84" s="4" t="s">
-        <v>124</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J85" s="4" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="K85" s="4" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J86" s="4" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="K86" s="4" t="s">
-        <v>111</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="10:11" s="4" customFormat="1" ht="25">
+      <c r="J87" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K87" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B5:H18">
     <cfRule type="cellIs" dxfId="2" priority="0" stopIfTrue="1" operator="equal">
@@ -1852,7 +1722,7 @@
       <formula>1</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="0" stopIfTrue="1" operator="equal">
-      <formula>" "</formula>
+      <formula>""" """</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
revised the extended Latin fonts for Hellscreiber
</commit_message>
<xml_diff>
--- a/fontmaker.xlsx
+++ b/fontmaker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="340" windowWidth="16500" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="16360" windowHeight="16400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,406 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+  <si>
+    <t>00000000000000-00111111101100-00000011000110-00000110001100-00001100000110-00111111100000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111000000000-00110000001100-00110000000110-00110000001100-00111111100000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111000110000-00111100110000-00110110111100-00110011110110-00110001110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111000110000-00111100110110-00110110110110-00110011110000-00110001110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00011111100000-00110000110110-00110000110000-00110000110110-00011111100000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00011111000000-00110001100000-00110001101100-00110001100110-00011111000000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-01111111111000-00111100001100-00110011001100-00110000111100-00011111111110-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111100-00001100110000-00001100110000-00001111110000-00000111100000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111110000-00110000000110-00110000000000-00110000000110-00111111110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111110000-00110000000110-00110000001100-00110000000110-00111111110000-00000000000000</t>
+  </si>
+  <si>
+    <t>(</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000000000000-00000000000000-00000111100000-00001111110000-00011000011000-00110000001100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00110000001100-00011000011000-00001111110000-00000111100000-00000000000000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111000110-00001101101100-00001100110000-00001101100000-00111111000000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111000000-00001101101100-00001100110110-00001101101100-00111111000000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111110000-00000011001100-00111111111100-00100011000100-00100011000100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111000-00000011001100-00000011001100-00111111111000-01100000000000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111100-00110000001100-00110000001100-01110000001100-00110000001100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111100000-00110001101100-00110001100110-00110001101100-00110001100000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111100000-00110001100000-00110001101100-00110001100110-00110001100000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111110000-00110000110110-00110000110110-00110110110110-00111110110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00110011100000-00110110111100-00110110110110-00110110111100-00011100110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00110011100000-00110110110110-00110110111100-00110110110110-00011100110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00110011100000-00110110110000-00110110111100-00110110110110-00011100110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111110000-00110110110000-00110110111100-00110110110110-00110110110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111110000-00110110110110-00110110111100-00110110110000-00110110110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00110011001100-00111111111100-00110011001100-00110000001100-00011111111000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00000110000000-00111111111100-00110011000000-00110000000000-00110000000000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111100-00110011001100-00110011001100-01110011001100-00110000001100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111100000-00000110001100-00000110000110-00000110001100-00111111100000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111100000-00000011000000-00000110001100-00001100000110-00111111100000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00110000001100-00111111111100-00110000001100-0000000001100-00000000011100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111111100-00001110000000-00000011100000-00000000111000-00111111111100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111110000-00011000000110-00000110001100-00000001100110-00111111110000-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-01111000000000-001101110001100-00110000111100-00111111111100-01110000001100-00000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Types a 1 or 0 into the grid below; 1 becomes a black pixel and zero a while pixel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copy result from above cell, then paste-special-value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Р</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>С</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Х</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ш</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Щ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ь</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Э</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ю</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Я</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Т</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>У</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ъ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ы</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^^</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comma</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>period</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>А</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Б</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Г</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Й</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>К</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>М</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latin M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Н</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ä</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Æ</t>
+  </si>
+  <si>
+    <t>Ą</t>
+  </si>
+  <si>
+    <t>À</t>
+  </si>
+  <si>
+    <t>Å</t>
+  </si>
+  <si>
+    <t>Ç</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ĉ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ć</t>
+  </si>
+  <si>
+    <t>Š</t>
+  </si>
+  <si>
+    <t>Ð</t>
+  </si>
+  <si>
+    <t>Ś</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>È</t>
+  </si>
+  <si>
+    <t>Ł</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>É</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ę</t>
+  </si>
+  <si>
+    <t>Ĝ</t>
+  </si>
+  <si>
+    <t>Ĥ</t>
+  </si>
+  <si>
+    <t>Ĵ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ź</t>
+  </si>
+  <si>
+    <t>Ñ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ö</t>
+  </si>
+  <si>
+    <t>Ó</t>
+  </si>
+  <si>
+    <t>Þ</t>
+  </si>
+  <si>
+    <t>Ü</t>
+  </si>
+  <si>
+    <t>Ŭ</t>
+  </si>
+  <si>
+    <t>Ż</t>
+  </si>
+  <si>
+    <t>Ń</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ø</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ŝ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>В</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Е</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ж</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>З</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>И</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Л</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>О</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>П</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ц</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000000000000-00111100111100-00000011000000-00111111111100-00000011000000-00111100111100-00000000000000</t>
+  </si>
+  <si>
+    <t>00000000000000-00111111000000-00001101100110-00001100110000-00001101100110-00111111000000-00000000000000</t>
+  </si>
   <si>
     <t>00000000000000-00000000001100-00000000001100-00111111111100-00110011000000-00011110000000-00000000000000</t>
   </si>
@@ -82,304 +481,6 @@
   </si>
   <si>
     <t>00000000000000-00110000001100-00111111111100-00110011001100-00110011001100-00011110001100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00110000001100-00111111111100-00110000001100-0000000001100-00000000011100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00111111111100-00001110000000-00000011100000-00000000111000-00111111111100-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-00111111110000-00011000000110-00000110001100-00000001100110-00111111110000-00000000000000</t>
-  </si>
-  <si>
-    <t>00000000000000-01111000000000-001101110001100-00110000111100-00111111111100-01110000001100-00000000000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Types a 1 or 0 into the grid below; 1 becomes a black pixel and zero a while pixel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Copy result from above cell, then paste-special-value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Р</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin P</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>С</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Х</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ш</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Щ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ь</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Э</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ю</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Я</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Т</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>У</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ъ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ы</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^^</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>comma</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>period</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>А</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Б</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Г</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Й</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>К</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin K</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>М</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latin M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Н</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ä</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Æ</t>
-  </si>
-  <si>
-    <t>Ą</t>
-  </si>
-  <si>
-    <t>À</t>
-  </si>
-  <si>
-    <t>Å</t>
-  </si>
-  <si>
-    <t>Ç</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ĉ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ć</t>
-  </si>
-  <si>
-    <t>Š</t>
-  </si>
-  <si>
-    <t>Ð</t>
-  </si>
-  <si>
-    <t>Ś</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>È</t>
-  </si>
-  <si>
-    <t>Ł</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>É</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ę</t>
-  </si>
-  <si>
-    <t>Ĝ</t>
-  </si>
-  <si>
-    <t>Ĥ</t>
-  </si>
-  <si>
-    <t>Ĵ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ź</t>
-  </si>
-  <si>
-    <t>Ñ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ö</t>
-  </si>
-  <si>
-    <t>Ó</t>
-  </si>
-  <si>
-    <t>Þ</t>
-  </si>
-  <si>
-    <t>Ü</t>
-  </si>
-  <si>
-    <t>Ŭ</t>
-  </si>
-  <si>
-    <t>Ż</t>
-  </si>
-  <si>
-    <t>Ń</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ø</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ŝ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>В</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Е</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ж</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>З</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>И</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Л</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>О</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>П</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ц</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00000000000000-00111100111100-00000011000000-00111111111100-00000011000000-00111100111100-00000000000000</t>
   </si>
 </sst>
 </file>
@@ -444,38 +545,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="8"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -832,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K87"/>
+  <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A65" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K79" sqref="K79"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A86" zoomScale="125" workbookViewId="0">
+      <selection activeCell="L100" sqref="L100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -846,7 +916,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -873,7 +943,7 @@
       </c>
       <c r="J3" s="2" t="str">
         <f>B21&amp;"-"&amp;C21&amp;"-"&amp;D21&amp;"-"&amp;E21&amp;"-"&amp;F21&amp;"-"&amp;G21&amp;"-"&amp;H21</f>
-        <v>00000000000000-00000000111100-00000001100000-00000001100000-00000001100000-00111111111100-00000000000000</v>
+        <v>00000000000000-00110000001100-00011000011000-00001111110000-00000111100000-00000000000000-00000000000000</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -885,7 +955,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -914,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -963,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -980,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -989,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1003,19 +1073,19 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1029,10 +1099,10 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1041,7 +1111,7 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1058,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1067,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1087,13 +1157,13 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1113,13 +1183,13 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1136,16 +1206,16 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1159,10 +1229,10 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1171,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1185,7 +1255,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1197,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1271,23 +1341,23 @@
       </c>
       <c r="C21" s="3" t="str">
         <f t="shared" ref="C21:H21" si="0">C18&amp;C17&amp;C16&amp;C15&amp;C14&amp;C13&amp;C12&amp;C11&amp;C10&amp;C9&amp;C8&amp;C7&amp;C6&amp;C5</f>
-        <v>00000000111100</v>
+        <v>00110000001100</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>00000001100000</v>
+        <v>00011000011000</v>
       </c>
       <c r="E21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>00000001100000</v>
+        <v>00001111110000</v>
       </c>
       <c r="F21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>00000001100000</v>
+        <v>00000111100000</v>
       </c>
       <c r="G21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>00111111111100</v>
+        <v>00000000000000</v>
       </c>
       <c r="H21" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1296,420 +1366,523 @@
     </row>
     <row r="24" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J24" s="4" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J25" s="4" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J26" s="4" t="s">
-        <v>61</v>
+        <v>73</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J27" s="4" t="s">
-        <v>62</v>
+        <v>74</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J28" s="4" t="s">
-        <v>63</v>
+        <v>75</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J29" s="4" t="s">
-        <v>64</v>
+        <v>76</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J30" s="4" t="s">
-        <v>65</v>
+        <v>77</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J31" s="4" t="s">
-        <v>66</v>
+        <v>78</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="4" customFormat="1" ht="25">
       <c r="J32" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>79</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J33" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>80</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J34" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>81</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J35" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>82</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J36" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>83</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J37" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>84</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J38" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>85</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J39" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>86</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J40" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>87</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J41" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>88</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J42" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>89</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J43" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>90</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J44" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>91</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J45" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>99</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J46" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>92</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J47" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="48" spans="10:10" s="4" customFormat="1" ht="25">
+        <v>93</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J48" s="4" t="s">
-        <v>88</v>
+        <v>100</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J49" s="4" t="s">
-        <v>82</v>
+        <v>94</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J50" s="4" t="s">
-        <v>89</v>
+        <v>101</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J51" s="4" t="s">
-        <v>83</v>
+        <v>95</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J52" s="4" t="s">
-        <v>84</v>
+        <v>96</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J53" s="4" t="s">
-        <v>85</v>
+        <v>97</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J54" s="4" t="s">
-        <v>86</v>
+        <v>98</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="10:11" s="4" customFormat="1" ht="25"/>
     <row r="56" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J56" s="4" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J57" s="4" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>19</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J58" s="4" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J59" s="4" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J60" s="4" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J61" s="4" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J62" s="4" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J63" s="4" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J64" s="4" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J65" s="4" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J66" s="4" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J67" s="4" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J68" s="4" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="K68" s="4" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J69" s="4" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="K69" s="4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J70" s="4" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="K70" s="4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J71" s="4" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
     </row>
     <row r="72" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J72" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="K72" s="4" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J73" s="4" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="K73" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="74" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J74" s="4" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="K74" s="4" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J75" s="4" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="K75" s="4" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J76" s="4" t="s">
-        <v>2</v>
+        <v>115</v>
       </c>
       <c r="K76" s="4" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J77" s="4" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="K77" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="78" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J78" s="4" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="K78" s="4" t="s">
-        <v>14</v>
+        <v>127</v>
       </c>
     </row>
     <row r="79" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J79" s="4" t="s">
-        <v>5</v>
+        <v>118</v>
       </c>
       <c r="K79" s="4" t="s">
-        <v>6</v>
+        <v>119</v>
       </c>
     </row>
     <row r="80" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J80" s="4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="K80" s="4" t="s">
-        <v>16</v>
+        <v>129</v>
       </c>
     </row>
     <row r="81" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J81" s="4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="K81" s="4" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J82" s="4" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="K82" s="4" t="s">
-        <v>0</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J83" s="4" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="K83" s="4" t="s">
-        <v>1</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J84" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="K84" s="4" t="s">
-        <v>7</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J85" s="4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="K85" s="4" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
     </row>
     <row r="86" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J86" s="4" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="K86" s="4" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
     </row>
     <row r="87" spans="10:11" s="4" customFormat="1" ht="25">
       <c r="J87" s="4" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="K87" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="10:11" ht="25">
+      <c r="J89" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="K89" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="10:11" ht="25">
+      <c r="J90" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K90" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>